<commit_message>
feat: :sparkles: add new features
</commit_message>
<xml_diff>
--- a/public/files/Formato.xlsx
+++ b/public/files/Formato.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oampe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAMP\htdocs\readybook-frontend\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A8A4CEF-6DFC-46D8-8281-A7464BF16586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D552570C-42C4-4BB8-9AFD-BA1F267169E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{241AFD19-1987-4DC9-A069-C7AA56529F6F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{241AFD19-1987-4DC9-A069-C7AA56529F6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>DPI</t>
+    <t>NOMBRE COMPLETO</t>
   </si>
   <si>
-    <t>NOMBRE COMPLETO</t>
+    <t>DPI / PASAPORTE</t>
+  </si>
+  <si>
+    <t>EDAD</t>
+  </si>
+  <si>
+    <t>GENERO</t>
+  </si>
+  <si>
+    <t>PAIS DE ORIGEN</t>
   </si>
 </sst>
 </file>
@@ -90,12 +99,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,24 +423,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED71C46A-CD63-48B5-9D80-522C946ABB7A}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="4"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>